<commit_message>
adding more code to the dirs
</commit_message>
<xml_diff>
--- a/twitter_scrap.xlsx
+++ b/twitter_scrap.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
   <si>
     <t>Username</t>
   </si>
@@ -34,22 +34,22 @@
     <t>Text</t>
   </si>
   <si>
-    <t>['يَعقوبْ قَمَرْ الدينْ ديبيازا repostado', 'gato preto']</t>
-  </si>
-  <si>
-    <t>258</t>
-  </si>
-  <si>
-    <t>1.812</t>
-  </si>
-  <si>
-    <t>12,1 mil</t>
-  </si>
-  <si>
-    <t>773,2 mil</t>
-  </si>
-  <si>
-    <t>· 16 h ele: ué cade minha porra q estava dentro da camisinha  eu na cozinha fazendo folha de papel com a porra dele pra escrevermos nossos votos de casamento Learn Something @cooltechtipz · 19 h Traditional way of making papers  0:16 258</t>
+    <t>['Naty está encantada', '@fadadesaturno']</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>77</t>
+  </si>
+  <si>
+    <t>1.688</t>
+  </si>
+  <si>
+    <t>28 mil</t>
+  </si>
+  <si>
+    <t>24 de ago Meu pai sempre apoiou meu sonho de ser escritora, e hoje tirei uma foto LINDA dele com meu livro!!! 30</t>
   </si>
 </sst>
 </file>
@@ -407,7 +407,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -453,6 +453,26 @@
         <v>11</v>
       </c>
     </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add a email sender function
</commit_message>
<xml_diff>
--- a/twitter_scrap.xlsx
+++ b/twitter_scrap.xlsx
@@ -34,22 +34,22 @@
     <t>Text</t>
   </si>
   <si>
-    <t>['Naty está encantada', '@fadadesaturno']</t>
-  </si>
-  <si>
-    <t>30</t>
-  </si>
-  <si>
-    <t>77</t>
-  </si>
-  <si>
-    <t>1.688</t>
-  </si>
-  <si>
-    <t>28 mil</t>
-  </si>
-  <si>
-    <t>24 de ago Meu pai sempre apoiou meu sonho de ser escritora, e hoje tirei uma foto LINDA dele com meu livro!!! 30</t>
+    <t>['Assanhando Livros |', '@assanhandolivro']</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>751</t>
+  </si>
+  <si>
+    <t>52,2 mil</t>
+  </si>
+  <si>
+    <t>22 de ago Não tem nada melhor que livro com rico apaixonado e vou provar:   Ela foi traída pelo noivo e numa viagem para superar o chifre acaba conhecendo um cara rico num passeio (não fazendo ideia que ele seja) viram amigos e conforme os dias vão passando ele lhe oferece um acordo... + 13</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
now using json to storage data
</commit_message>
<xml_diff>
--- a/twitter_scrap.xlsx
+++ b/twitter_scrap.xlsx
@@ -34,22 +34,22 @@
     <t>Text</t>
   </si>
   <si>
-    <t>['Assanhando Livros |', '@assanhandolivro']</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>42</t>
-  </si>
-  <si>
-    <t>751</t>
-  </si>
-  <si>
-    <t>52,2 mil</t>
-  </si>
-  <si>
-    <t>22 de ago Não tem nada melhor que livro com rico apaixonado e vou provar:   Ela foi traída pelo noivo e numa viagem para superar o chifre acaba conhecendo um cara rico num passeio (não fazendo ideia que ele seja) viram amigos e conforme os dias vão passando ele lhe oferece um acordo... + 13</t>
+    <t>['cozy // Alex Claremont', '@alxclaremont']</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>101</t>
+  </si>
+  <si>
+    <t>1.966</t>
+  </si>
+  <si>
+    <t>8 de set Alex se formou então na sequência teremos Alex advogado e Henry escritor e se o Henry escrever a história deles ??????????????????? Se vbsa livro for referênciado como Henry autor $^&amp;$#@+×#$$%_^&amp; 9</t>
   </si>
 </sst>
 </file>

</xml_diff>